<commit_message>
All cleaned up, just need to edit acknowledgements
</commit_message>
<xml_diff>
--- a/data/Table3_2.xlsx
+++ b/data/Table3_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebatz\Documents\Dissertation\Batzer_Dissertation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D52D17C-A9F0-4C4C-91DA-2A969494D0E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25583FB7-DC89-4EEF-9A56-EAE1C34DAEE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5347" yWindow="2509" windowWidth="20530" windowHeight="12076" xr2:uid="{92E9C512-7C64-4B38-A9F5-61AAE272D99C}"/>
+    <workbookView xWindow="1839" yWindow="2010" windowWidth="20531" windowHeight="10793" xr2:uid="{92E9C512-7C64-4B38-A9F5-61AAE272D99C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Temporal Priority</t>
-  </si>
-  <si>
     <t>Drought Stress (SPEI)</t>
   </si>
   <si>
@@ -146,13 +143,16 @@
     <t>0.73 (0.65,0.79)</t>
   </si>
   <si>
-    <t>3.31`</t>
-  </si>
-  <si>
-    <t>4.77`</t>
-  </si>
-  <si>
-    <t>0.55`</t>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>4.77'</t>
+  </si>
+  <si>
+    <t>3.31'</t>
+  </si>
+  <si>
+    <t>0.55'</t>
   </si>
 </sst>
 </file>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D3106B-29C0-46D1-8147-DDD9F7926EF9}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -655,41 +655,41 @@
         <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1">
         <v>0.8</v>
@@ -698,10 +698,10 @@
     <row r="5" spans="1:6" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="5">
         <v>2.96</v>
@@ -713,10 +713,10 @@
     <row r="6" spans="1:6" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="12">
         <v>1.53</v>
@@ -727,16 +727,16 @@
     </row>
     <row r="7" spans="1:6" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1">
         <v>0.83</v>
@@ -744,30 +744,30 @@
     </row>
     <row r="8" spans="1:6" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="5">
         <v>1.71</v>
@@ -779,10 +779,10 @@
     <row r="10" spans="1:6" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="12">
         <v>0.54</v>
@@ -793,30 +793,30 @@
     </row>
     <row r="11" spans="1:6" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="E11" s="14" t="s">
         <v>24</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="5">
         <v>0.55000000000000004</v>
@@ -828,59 +828,59 @@
     <row r="13" spans="1:6" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>29</v>
-      </c>
       <c r="E14" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="E15" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25.7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="5">
         <v>0.77</v>
@@ -892,10 +892,10 @@
     <row r="17" spans="1:5" ht="15.7" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="5">
         <v>1.93</v>
@@ -907,16 +907,16 @@
     <row r="18" spans="1:5" ht="16.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>